<commit_message>
add Presence database- arrival & departure functions
</commit_message>
<xml_diff>
--- a/workOnExcel/Constraints1.xlsx
+++ b/workOnExcel/Constraints1.xlsx
@@ -7,18 +7,20 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="michal" sheetId="1" r:id="rId1"/>
-    <sheet name="shir" sheetId="2" r:id="rId2"/>
-    <sheet name="emilia" sheetId="3" r:id="rId3"/>
-    <sheet name="emilia&amp;shir" sheetId="4" r:id="rId4"/>
-    <sheet name="kakaka" sheetId="5" r:id="rId5"/>
+    <sheet name="adir" sheetId="1" r:id="rId1"/>
+    <sheet name="stav" sheetId="2" r:id="rId2"/>
+    <sheet name="tair" sheetId="3" r:id="rId3"/>
+    <sheet name="yoni" sheetId="4" r:id="rId4"/>
+    <sheet name="asaf" sheetId="5" r:id="rId5"/>
+    <sheet name="rotem" sheetId="6" r:id="rId6"/>
+    <sheet name="michal" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="10">
   <si>
     <t>Sunday</t>
   </si>
@@ -415,16 +417,10 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
@@ -470,7 +466,7 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="H2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -478,7 +474,7 @@
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
+      <c r="F3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -522,15 +518,15 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -577,13 +573,13 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -629,13 +625,117 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add the option of making shifts, manager 11 option in menu
</commit_message>
<xml_diff>
--- a/workOnExcel/Constraints1.xlsx
+++ b/workOnExcel/Constraints1.xlsx
@@ -7,20 +7,27 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="adir" sheetId="1" r:id="rId1"/>
-    <sheet name="stav" sheetId="2" r:id="rId2"/>
-    <sheet name="tair" sheetId="3" r:id="rId3"/>
-    <sheet name="yoni" sheetId="4" r:id="rId4"/>
-    <sheet name="asaf" sheetId="5" r:id="rId5"/>
-    <sheet name="rotem" sheetId="6" r:id="rId6"/>
-    <sheet name="michal" sheetId="7" r:id="rId7"/>
+    <sheet name="shifts" sheetId="1" r:id="rId1"/>
+    <sheet name="adir" sheetId="2" r:id="rId2"/>
+    <sheet name="stav" sheetId="3" r:id="rId3"/>
+    <sheet name="tair" sheetId="4" r:id="rId4"/>
+    <sheet name="yoni" sheetId="5" r:id="rId5"/>
+    <sheet name="asaf" sheetId="6" r:id="rId6"/>
+    <sheet name="rotem" sheetId="7" r:id="rId7"/>
+    <sheet name="michal" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="17">
+  <si>
+    <t>Morning</t>
+  </si>
+  <si>
+    <t>Evening</t>
+  </si>
   <si>
     <t>Sunday</t>
   </si>
@@ -43,13 +50,28 @@
     <t>Saturday</t>
   </si>
   <si>
-    <t>Morning</t>
+    <t>rotem</t>
+  </si>
+  <si>
+    <t>tair</t>
+  </si>
+  <si>
+    <t>asaf</t>
+  </si>
+  <si>
+    <t>yoni</t>
+  </si>
+  <si>
+    <t>stav</t>
+  </si>
+  <si>
+    <t>michal</t>
+  </si>
+  <si>
+    <t>adir</t>
   </si>
   <si>
     <t>NO</t>
-  </si>
-  <si>
-    <t>Evening</t>
   </si>
 </sst>
 </file>
@@ -381,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -389,41 +411,117 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
-        <v>8</v>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -441,41 +539,41 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -493,41 +591,41 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -545,41 +643,41 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -597,41 +695,41 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -649,41 +747,41 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" t="s">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -701,41 +799,93 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>